<commit_message>
:bug: Fix copy sheet error
</commit_message>
<xml_diff>
--- a/sample/copy-sheet/src1.xlsx
+++ b/sample/copy-sheet/src1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t>基本信息</t>
   </si>
@@ -68,6 +68,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="5"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>种</t>
@@ -76,16 +77,87 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>文字</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
   </si>
   <si>
     <t>余雨彤</t>
   </si>
   <si>
+    <r>
+      <t>多</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>种</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
     <t>杜恺玲</t>
+  </si>
+  <si>
+    <r>
+      <t>多</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>种</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="28"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
   </si>
   <si>
     <t>黄清昶</t>
@@ -102,12 +174,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,6 +225,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -167,6 +245,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -175,26 +260,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -208,82 +278,59 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,10 +344,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="5"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -319,61 +403,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,115 +577,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,6 +600,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -527,36 +620,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -596,11 +659,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -609,152 +693,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -778,6 +862,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1101,7 +1188,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="6"/>
@@ -1251,11 +1338,11 @@
       <c r="C13">
         <v>33</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" ht="18" spans="1:7">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1265,16 +1352,22 @@
       <c r="C14">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="G14" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" ht="40" spans="1:7">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>27</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1282,7 +1375,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -1293,7 +1386,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>28</v>
@@ -1301,7 +1394,7 @@
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <f>SUM(C3:C17)</f>

</xml_diff>